<commit_message>
modif nom des variables
</commit_message>
<xml_diff>
--- a/Donnees_CREPS_1.xlsx
+++ b/Donnees_CREPS_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexia\Desktop\INSA\4A\PROJET\Projet_CREPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e3e93a7e0c88a78/Documents/INSA_4_GMM/Semestre 2/Projet tutoré/Projet_CREPS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138B9CAC-AAA8-4D00-B99F-C23CB635B132}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{138B9CAC-AAA8-4D00-B99F-C23CB635B132}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FAD586DA-47D9-4582-8AF9-F5971A667D1B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees_CREPS_1" sheetId="1" r:id="rId1"/>
@@ -335,64 +335,64 @@
     <t>COLETTE HUGO</t>
   </si>
   <si>
-    <t xml:space="preserve">Adductor stretch </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hamstring stretch G </t>
-  </si>
-  <si>
-    <t>Hamstring Stretch D</t>
-  </si>
-  <si>
-    <t>Quad Stretch G</t>
-  </si>
-  <si>
-    <t>Quad Stretch D</t>
-  </si>
-  <si>
-    <t>Pigeon Posé G</t>
-  </si>
-  <si>
-    <t>Pigeon Posé D</t>
-  </si>
-  <si>
     <t>Chandelier</t>
   </si>
   <si>
-    <t>Arm Clock G</t>
-  </si>
-  <si>
-    <t>Arm Clock D</t>
-  </si>
-  <si>
-    <t>Reverse table</t>
-  </si>
-  <si>
-    <t>Overhead Squat</t>
-  </si>
-  <si>
-    <t>Hurdle step D</t>
-  </si>
-  <si>
-    <t>Hurdle step G</t>
-  </si>
-  <si>
-    <t>Hamstring curl G</t>
-  </si>
-  <si>
-    <t>Hamstring Curl D</t>
-  </si>
-  <si>
-    <t>Copenhagen plank G</t>
-  </si>
-  <si>
-    <t>Copenhagen D</t>
-  </si>
-  <si>
-    <t>Push Up</t>
-  </si>
-  <si>
-    <t>Core Activation</t>
+    <t xml:space="preserve">AdductorStretch </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HamstringStretchG </t>
+  </si>
+  <si>
+    <t>HamstringStretchD</t>
+  </si>
+  <si>
+    <t>QuadStretchG</t>
+  </si>
+  <si>
+    <t>QuadStretchD</t>
+  </si>
+  <si>
+    <t>PigeonPoseG</t>
+  </si>
+  <si>
+    <t>PigeonPoseD</t>
+  </si>
+  <si>
+    <t>ArmClockG</t>
+  </si>
+  <si>
+    <t>ArmClockD</t>
+  </si>
+  <si>
+    <t>ReverseTable</t>
+  </si>
+  <si>
+    <t>OverheadSquat</t>
+  </si>
+  <si>
+    <t>HurdleStepG</t>
+  </si>
+  <si>
+    <t>HurdleStepD</t>
+  </si>
+  <si>
+    <t>HamstringCurlG</t>
+  </si>
+  <si>
+    <t>HamstringCurlD</t>
+  </si>
+  <si>
+    <t>CopenhagenPlankG</t>
+  </si>
+  <si>
+    <t>CopenhagenD</t>
+  </si>
+  <si>
+    <t>PushUp</t>
+  </si>
+  <si>
+    <t>CoreActivation</t>
   </si>
 </sst>
 </file>
@@ -1236,13 +1236,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -1265,28 +1265,28 @@
         <v>97</v>
       </c>
       <c r="H1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L1" t="s">
+        <v>106</v>
+      </c>
+      <c r="M1" t="s">
+        <v>107</v>
+      </c>
+      <c r="N1" t="s">
+        <v>108</v>
+      </c>
+      <c r="O1" t="s">
         <v>101</v>
-      </c>
-      <c r="I1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J1" t="s">
-        <v>103</v>
-      </c>
-      <c r="K1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L1" t="s">
-        <v>105</v>
-      </c>
-      <c r="M1" t="s">
-        <v>106</v>
-      </c>
-      <c r="N1" t="s">
-        <v>107</v>
-      </c>
-      <c r="O1" t="s">
-        <v>108</v>
       </c>
       <c r="P1" t="s">
         <v>109</v>
@@ -1301,10 +1301,10 @@
         <v>112</v>
       </c>
       <c r="T1" t="s">
+        <v>113</v>
+      </c>
+      <c r="U1" t="s">
         <v>114</v>
-      </c>
-      <c r="U1" t="s">
-        <v>113</v>
       </c>
       <c r="V1" t="s">
         <v>115</v>
@@ -1325,7 +1325,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1413,12 +1413,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B5" si="0">D3+E3+F3+G3</f>
+        <f t="shared" ref="B3:B4" si="0">D3+E3+F3+G3</f>
         <v>12</v>
       </c>
       <c r="C3" t="s">
@@ -1501,7 +1501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1677,12 +1677,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B3:B66" si="5">D6+E6+F6+G6</f>
+        <f t="shared" ref="B6:B66" si="5">D6+E6+F6+G6</f>
         <v>10</v>
       </c>
       <c r="C6" t="s">
@@ -1765,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -4757,7 +4757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -5197,7 +5197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -5461,7 +5461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -5725,7 +5725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -5901,7 +5901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -5989,7 +5989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -6077,7 +6077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -6165,7 +6165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -6253,7 +6253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -6341,7 +6341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -6429,7 +6429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -6517,7 +6517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -6605,7 +6605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -6693,7 +6693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -6781,7 +6781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -6869,7 +6869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -6957,7 +6957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -7045,19 +7045,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>68</v>
       </c>
       <c r="B67">
-        <f t="shared" ref="B67:B91" si="6">D67+E67+F67+G67</f>
+        <f t="shared" ref="B67:B89" si="6">D67+E67+F67+G67</f>
         <v>8</v>
       </c>
       <c r="C67" t="s">
         <v>99</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D91" si="7">H67+I67+J67+K67+L67+M67+N67+S67</f>
+        <f t="shared" ref="D67:D89" si="7">H67+I67+J67+K67+L67+M67+N67+S67</f>
         <v>1</v>
       </c>
       <c r="E67">
@@ -7065,11 +7065,11 @@
         <v>2</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F91" si="9">T67+U67+V67+W67+X67+Y67</f>
+        <f t="shared" ref="F67:F89" si="9">T67+U67+V67+W67+X67+Y67</f>
         <v>4</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G92" si="10">Z67+AA67</f>
+        <f t="shared" ref="G67:G89" si="10">Z67+AA67</f>
         <v>1</v>
       </c>
       <c r="H67">
@@ -7133,7 +7133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -7221,7 +7221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>71</v>
       </c>
@@ -7397,7 +7397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>100</v>
       </c>
@@ -7425,7 +7425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -7513,7 +7513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -7601,7 +7601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -7689,7 +7689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -7777,7 +7777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -7865,7 +7865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -7953,7 +7953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -8041,7 +8041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -8129,7 +8129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -8217,7 +8217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -8305,7 +8305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -8393,7 +8393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -8481,7 +8481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -8569,7 +8569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>85</v>
       </c>
@@ -8657,7 +8657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>86</v>
       </c>
@@ -8745,7 +8745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -8833,7 +8833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -8921,7 +8921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -8937,7 +8937,7 @@
         <v>0</v>
       </c>
       <c r="E89">
-        <f t="shared" ref="E89:E91" si="11">O89+P89+Q89+R89</f>
+        <f t="shared" ref="E89" si="11">O89+P89+Q89+R89</f>
         <v>4</v>
       </c>
       <c r="F89">

</xml_diff>

<commit_message>
Tests de student et modif excel
</commit_message>
<xml_diff>
--- a/Donnees_CREPS_1.xlsx
+++ b/Donnees_CREPS_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e3e93a7e0c88a78/Documents/INSA_4_GMM/Semestre 2/Projet tutoré/Projet_CREPS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{138B9CAC-AAA8-4D00-B99F-C23CB635B132}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FAD586DA-47D9-4582-8AF9-F5971A667D1B}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{138B9CAC-AAA8-4D00-B99F-C23CB635B132}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{60860B35-37A4-4230-94B5-680AB9956754}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1236,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7403,25 +7403,85 @@
       </c>
       <c r="B71">
         <f>D71+E71+F71+G71</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C71" t="s">
         <v>99</v>
       </c>
       <c r="D71">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F71">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G71">
         <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>1</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
+      </c>
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="Q71">
+        <v>0</v>
+      </c>
+      <c r="R71">
+        <v>1</v>
+      </c>
+      <c r="S71">
+        <v>0</v>
+      </c>
+      <c r="T71">
+        <v>1</v>
+      </c>
+      <c r="U71">
+        <v>1</v>
+      </c>
+      <c r="V71">
+        <v>0</v>
+      </c>
+      <c r="W71">
+        <v>0</v>
+      </c>
+      <c r="X71">
+        <v>1</v>
+      </c>
+      <c r="Y71">
+        <v>1</v>
+      </c>
+      <c r="Z71">
+        <v>1</v>
+      </c>
+      <c r="AA71">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ajouts Baseball et Rugby, enfin !
</commit_message>
<xml_diff>
--- a/Donnees_CREPS_1.xlsx
+++ b/Donnees_CREPS_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e3e93a7e0c88a78/Documents/INSA_4_GMM/Semestre 2/Projet tutoré/Projet_CREPS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexia\Desktop\INSA\4A\PROJET\Projet_CREPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{138B9CAC-AAA8-4D00-B99F-C23CB635B132}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FAD586DA-47D9-4582-8AF9-F5971A667D1B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6816287-26AE-48B7-83C5-A2DA5F68D6B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4940" yWindow="820" windowWidth="14400" windowHeight="9160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees_CREPS_1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="158">
   <si>
     <t>SCORE</t>
   </si>
@@ -393,6 +393,117 @@
   </si>
   <si>
     <t>CoreActivation</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>LIPPERT MATHIS</t>
+  </si>
+  <si>
+    <t>LACOMBE MATHIAS</t>
+  </si>
+  <si>
+    <t>NAYRAL MATHIS</t>
+  </si>
+  <si>
+    <t>LOUCEAUD ICOSTA</t>
+  </si>
+  <si>
+    <t>BOMBERGER KYLIAN</t>
+  </si>
+  <si>
+    <t>DOAT PIERRE</t>
+  </si>
+  <si>
+    <t>SALADO PABLO</t>
+  </si>
+  <si>
+    <t>MALLET ROMAIN</t>
+  </si>
+  <si>
+    <t>MERCADIER THIBAULT</t>
+  </si>
+  <si>
+    <t>BLANC VALENTIN</t>
+  </si>
+  <si>
+    <t>JAMOUS SAMY</t>
+  </si>
+  <si>
+    <t>BIDAUT ARTHUR</t>
+  </si>
+  <si>
+    <t>DEMORY THOMAS</t>
+  </si>
+  <si>
+    <t>HASSED FITMEH</t>
+  </si>
+  <si>
+    <t>ESPOSITO KENNY</t>
+  </si>
+  <si>
+    <t>PERROIS ARTHUR</t>
+  </si>
+  <si>
+    <t>BLANCOT BAPTISTE</t>
+  </si>
+  <si>
+    <t>TOUBEAUX JOSEPH</t>
+  </si>
+  <si>
+    <t>KEKENBOSH ETHAN</t>
+  </si>
+  <si>
+    <t>DOURET MAXENCE</t>
+  </si>
+  <si>
+    <t>ENRIANE THONAND NOAH</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>MAILLARD IMANOL</t>
+  </si>
+  <si>
+    <t>FLEURY NESTA</t>
+  </si>
+  <si>
+    <t>GAUTIER MARIUS</t>
+  </si>
+  <si>
+    <t>DANIEL LUCAS</t>
+  </si>
+  <si>
+    <t>GOFFIN BRADLEY</t>
+  </si>
+  <si>
+    <t>BARJOU ANTHONY</t>
+  </si>
+  <si>
+    <t>RODRIGUEZ BAPTISTE</t>
+  </si>
+  <si>
+    <t>SAVAR RAPHAEL</t>
+  </si>
+  <si>
+    <t>LAC YANNIS</t>
+  </si>
+  <si>
+    <t>BINDA VALENTIN</t>
+  </si>
+  <si>
+    <t>CRUNEL QUENTIN</t>
+  </si>
+  <si>
+    <t>CARRASCO TOM</t>
+  </si>
+  <si>
+    <t>ENNOYOTIE SOSTHENE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TROPIS ROMEO </t>
   </si>
 </sst>
 </file>
@@ -878,7 +989,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1234,15 +1345,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA89"/>
+  <dimension ref="A1:AA124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -1325,7 +1436,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1413,7 +1524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1501,7 +1612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1589,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1677,7 +1788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1765,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1853,7 +1964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1941,7 +2052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2029,7 +2140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2117,7 +2228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2205,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2293,7 +2404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2381,7 +2492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2469,7 +2580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2557,7 +2668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2645,7 +2756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -2733,7 +2844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2821,7 +2932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2909,7 +3020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2997,7 +3108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -3085,7 +3196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -3173,7 +3284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -3261,7 +3372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3349,7 +3460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -3437,7 +3548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -3525,7 +3636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -3613,7 +3724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -3701,7 +3812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -3789,7 +3900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -3877,7 +3988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -3965,7 +4076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -4053,7 +4164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -4141,7 +4252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -4229,7 +4340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -4317,7 +4428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -4405,7 +4516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -4493,7 +4604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -4581,7 +4692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -4669,7 +4780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -4757,7 +4868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -4845,7 +4956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -4933,7 +5044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -5021,7 +5132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -5109,7 +5220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -5197,7 +5308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -5285,7 +5396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -5373,7 +5484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -5461,7 +5572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -5549,7 +5660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -5637,7 +5748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -5725,7 +5836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -5813,7 +5924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -5901,7 +6012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -5989,7 +6100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -6077,7 +6188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -6165,7 +6276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -6253,7 +6364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -6341,7 +6452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -6429,7 +6540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -6517,7 +6628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -6605,7 +6716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -6693,7 +6804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -6781,7 +6892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -6869,7 +6980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -6957,7 +7068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -7045,19 +7156,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>68</v>
       </c>
       <c r="B67">
-        <f t="shared" ref="B67:B89" si="6">D67+E67+F67+G67</f>
+        <f t="shared" ref="B67:B124" si="6">D67+E67+F67+G67</f>
         <v>8</v>
       </c>
       <c r="C67" t="s">
         <v>99</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D89" si="7">H67+I67+J67+K67+L67+M67+N67+S67</f>
+        <f t="shared" ref="D67:D124" si="7">H67+I67+J67+K67+L67+M67+N67+S67</f>
         <v>1</v>
       </c>
       <c r="E67">
@@ -7065,11 +7176,11 @@
         <v>2</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F89" si="9">T67+U67+V67+W67+X67+Y67</f>
+        <f t="shared" ref="F67:F124" si="9">T67+U67+V67+W67+X67+Y67</f>
         <v>4</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G89" si="10">Z67+AA67</f>
+        <f t="shared" ref="G67:G124" si="10">Z67+AA67</f>
         <v>1</v>
       </c>
       <c r="H67">
@@ -7133,7 +7244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -7221,7 +7332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -7309,123 +7420,183 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>100</v>
+      </c>
+      <c r="B70" s="1">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="C70" t="s">
+        <v>99</v>
+      </c>
+      <c r="D70" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E70" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="F70" s="1">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G70" s="1">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H70" s="1">
+        <v>0</v>
+      </c>
+      <c r="I70" s="1">
+        <v>0</v>
+      </c>
+      <c r="J70" s="1">
+        <v>0</v>
+      </c>
+      <c r="K70" s="1">
+        <v>0</v>
+      </c>
+      <c r="L70" s="1">
+        <v>1</v>
+      </c>
+      <c r="M70" s="1">
+        <v>0</v>
+      </c>
+      <c r="N70" s="1">
+        <v>0</v>
+      </c>
+      <c r="O70" s="1">
+        <v>0</v>
+      </c>
+      <c r="P70" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q70" s="1">
+        <v>0</v>
+      </c>
+      <c r="R70" s="1">
+        <v>1</v>
+      </c>
+      <c r="S70" s="1">
+        <v>0</v>
+      </c>
+      <c r="T70" s="1">
+        <v>1</v>
+      </c>
+      <c r="U70" s="1">
+        <v>1</v>
+      </c>
+      <c r="V70" s="1">
+        <v>0</v>
+      </c>
+      <c r="W70" s="1">
+        <v>0</v>
+      </c>
+      <c r="X70" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y70" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z70" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA70" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>71</v>
       </c>
-      <c r="B70">
+      <c r="B71">
         <f t="shared" si="6"/>
         <v>11</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
         <v>99</v>
       </c>
-      <c r="D70">
+      <c r="D71">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="E70">
+      <c r="E71">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="F70">
+      <c r="F71">
         <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="G70">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="H70">
-        <v>1</v>
-      </c>
-      <c r="I70">
-        <v>0</v>
-      </c>
-      <c r="J70">
-        <v>0</v>
-      </c>
-      <c r="K70">
-        <v>0</v>
-      </c>
-      <c r="L70">
-        <v>0</v>
-      </c>
-      <c r="M70">
-        <v>1</v>
-      </c>
-      <c r="N70">
-        <v>0</v>
-      </c>
-      <c r="O70">
-        <v>1</v>
-      </c>
-      <c r="P70">
-        <v>1</v>
-      </c>
-      <c r="Q70">
-        <v>1</v>
-      </c>
-      <c r="R70">
-        <v>1</v>
-      </c>
-      <c r="S70">
-        <v>0</v>
-      </c>
-      <c r="T70">
-        <v>1</v>
-      </c>
-      <c r="U70">
-        <v>0</v>
-      </c>
-      <c r="V70">
-        <v>1</v>
-      </c>
-      <c r="W70">
-        <v>1</v>
-      </c>
-      <c r="X70">
-        <v>0</v>
-      </c>
-      <c r="Y70">
-        <v>1</v>
-      </c>
-      <c r="Z70">
-        <v>1</v>
-      </c>
-      <c r="AA70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B71">
-        <f>D71+E71+F71+G71</f>
-        <v>0</v>
-      </c>
-      <c r="C71" t="s">
-        <v>99</v>
-      </c>
-      <c r="D71">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E71">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F71">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
       <c r="G71">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>1</v>
+      </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <v>1</v>
+      </c>
+      <c r="P71">
+        <v>1</v>
+      </c>
+      <c r="Q71">
+        <v>1</v>
+      </c>
+      <c r="R71">
+        <v>1</v>
+      </c>
+      <c r="S71">
+        <v>0</v>
+      </c>
+      <c r="T71">
+        <v>1</v>
+      </c>
+      <c r="U71">
+        <v>0</v>
+      </c>
+      <c r="V71">
+        <v>1</v>
+      </c>
+      <c r="W71">
+        <v>1</v>
+      </c>
+      <c r="X71">
+        <v>0</v>
+      </c>
+      <c r="Y71">
+        <v>1</v>
+      </c>
+      <c r="Z71">
+        <v>1</v>
+      </c>
+      <c r="AA71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -7513,7 +7684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -7601,7 +7772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -7689,7 +7860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -7777,7 +7948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -7865,7 +8036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -7953,7 +8124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -8041,7 +8212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -8129,7 +8300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -8217,7 +8388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -8305,7 +8476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -8393,7 +8564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -8481,7 +8652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -8569,7 +8740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>85</v>
       </c>
@@ -8657,7 +8828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>86</v>
       </c>
@@ -8745,7 +8916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -8833,7 +9004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -8921,7 +9092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -8937,7 +9108,7 @@
         <v>0</v>
       </c>
       <c r="E89">
-        <f t="shared" ref="E89" si="11">O89+P89+Q89+R89</f>
+        <f t="shared" ref="E89:E124" si="11">O89+P89+Q89+R89</f>
         <v>4</v>
       </c>
       <c r="F89">
@@ -9007,6 +9178,3086 @@
       </c>
       <c r="AA89">
         <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>122</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="C90" t="s">
+        <v>121</v>
+      </c>
+      <c r="D90">
+        <f>H90+I90+J90+K90+L90+M90+N90+S90</f>
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+      <c r="J90">
+        <v>0</v>
+      </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
+      <c r="L90">
+        <v>0</v>
+      </c>
+      <c r="M90">
+        <v>0</v>
+      </c>
+      <c r="N90">
+        <v>0</v>
+      </c>
+      <c r="O90">
+        <v>0</v>
+      </c>
+      <c r="P90">
+        <v>0</v>
+      </c>
+      <c r="Q90">
+        <v>0</v>
+      </c>
+      <c r="R90">
+        <v>1</v>
+      </c>
+      <c r="S90">
+        <v>0</v>
+      </c>
+      <c r="T90">
+        <v>1</v>
+      </c>
+      <c r="U90">
+        <v>0</v>
+      </c>
+      <c r="V90">
+        <v>0</v>
+      </c>
+      <c r="W90">
+        <v>0</v>
+      </c>
+      <c r="X90">
+        <v>1</v>
+      </c>
+      <c r="Y90">
+        <v>1</v>
+      </c>
+      <c r="Z90">
+        <v>1</v>
+      </c>
+      <c r="AA90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>123</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="C91" t="s">
+        <v>121</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
+        <v>0</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+      <c r="K91">
+        <v>1</v>
+      </c>
+      <c r="L91">
+        <v>1</v>
+      </c>
+      <c r="M91">
+        <v>1</v>
+      </c>
+      <c r="N91">
+        <v>1</v>
+      </c>
+      <c r="O91">
+        <v>1</v>
+      </c>
+      <c r="P91">
+        <v>1</v>
+      </c>
+      <c r="Q91">
+        <v>1</v>
+      </c>
+      <c r="R91">
+        <v>1</v>
+      </c>
+      <c r="S91">
+        <v>1</v>
+      </c>
+      <c r="T91">
+        <v>1</v>
+      </c>
+      <c r="U91">
+        <v>1</v>
+      </c>
+      <c r="V91">
+        <v>1</v>
+      </c>
+      <c r="W91">
+        <v>1</v>
+      </c>
+      <c r="X91">
+        <v>0</v>
+      </c>
+      <c r="Y91">
+        <v>0</v>
+      </c>
+      <c r="Z91">
+        <v>1</v>
+      </c>
+      <c r="AA91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>124</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="C92" t="s">
+        <v>121</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="G92">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
+        <v>1</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+      <c r="K92">
+        <v>1</v>
+      </c>
+      <c r="L92">
+        <v>0</v>
+      </c>
+      <c r="M92">
+        <v>0</v>
+      </c>
+      <c r="N92">
+        <v>0</v>
+      </c>
+      <c r="O92">
+        <v>0</v>
+      </c>
+      <c r="P92">
+        <v>0</v>
+      </c>
+      <c r="Q92">
+        <v>0</v>
+      </c>
+      <c r="R92">
+        <v>1</v>
+      </c>
+      <c r="S92">
+        <v>0</v>
+      </c>
+      <c r="T92">
+        <v>0</v>
+      </c>
+      <c r="U92">
+        <v>0</v>
+      </c>
+      <c r="V92">
+        <v>0</v>
+      </c>
+      <c r="W92">
+        <v>1</v>
+      </c>
+      <c r="X92">
+        <v>1</v>
+      </c>
+      <c r="Y92">
+        <v>1</v>
+      </c>
+      <c r="Z92">
+        <v>1</v>
+      </c>
+      <c r="AA92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>125</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="C93" t="s">
+        <v>121</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="G93">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93">
+        <v>0</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
+      <c r="L93">
+        <v>0</v>
+      </c>
+      <c r="M93">
+        <v>0</v>
+      </c>
+      <c r="N93">
+        <v>0</v>
+      </c>
+      <c r="O93">
+        <v>0</v>
+      </c>
+      <c r="P93">
+        <v>0</v>
+      </c>
+      <c r="Q93">
+        <v>0</v>
+      </c>
+      <c r="R93">
+        <v>1</v>
+      </c>
+      <c r="S93">
+        <v>1</v>
+      </c>
+      <c r="T93">
+        <v>1</v>
+      </c>
+      <c r="U93">
+        <v>1</v>
+      </c>
+      <c r="V93">
+        <v>0</v>
+      </c>
+      <c r="W93">
+        <v>0</v>
+      </c>
+      <c r="X93">
+        <v>0</v>
+      </c>
+      <c r="Y93">
+        <v>1</v>
+      </c>
+      <c r="Z93">
+        <v>1</v>
+      </c>
+      <c r="AA93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>126</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="C94" t="s">
+        <v>121</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+      <c r="K94">
+        <v>1</v>
+      </c>
+      <c r="L94">
+        <v>0</v>
+      </c>
+      <c r="M94">
+        <v>0</v>
+      </c>
+      <c r="N94">
+        <v>0</v>
+      </c>
+      <c r="O94">
+        <v>1</v>
+      </c>
+      <c r="P94">
+        <v>0</v>
+      </c>
+      <c r="Q94">
+        <v>0</v>
+      </c>
+      <c r="R94">
+        <v>1</v>
+      </c>
+      <c r="S94">
+        <v>0</v>
+      </c>
+      <c r="T94">
+        <v>0</v>
+      </c>
+      <c r="U94">
+        <v>0</v>
+      </c>
+      <c r="V94">
+        <v>1</v>
+      </c>
+      <c r="W94">
+        <v>1</v>
+      </c>
+      <c r="X94">
+        <v>1</v>
+      </c>
+      <c r="Y94">
+        <v>1</v>
+      </c>
+      <c r="Z94">
+        <v>1</v>
+      </c>
+      <c r="AA94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>127</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="C95" t="s">
+        <v>121</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="G95">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
+      </c>
+      <c r="J95">
+        <v>0</v>
+      </c>
+      <c r="K95">
+        <v>1</v>
+      </c>
+      <c r="L95">
+        <v>1</v>
+      </c>
+      <c r="M95">
+        <v>0</v>
+      </c>
+      <c r="N95">
+        <v>0</v>
+      </c>
+      <c r="O95">
+        <v>0</v>
+      </c>
+      <c r="P95">
+        <v>0</v>
+      </c>
+      <c r="Q95">
+        <v>1</v>
+      </c>
+      <c r="R95">
+        <v>1</v>
+      </c>
+      <c r="S95">
+        <v>1</v>
+      </c>
+      <c r="T95">
+        <v>1</v>
+      </c>
+      <c r="U95">
+        <v>1</v>
+      </c>
+      <c r="V95">
+        <v>1</v>
+      </c>
+      <c r="W95">
+        <v>1</v>
+      </c>
+      <c r="X95">
+        <v>1</v>
+      </c>
+      <c r="Y95">
+        <v>1</v>
+      </c>
+      <c r="Z95">
+        <v>1</v>
+      </c>
+      <c r="AA95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>128</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="C96" t="s">
+        <v>121</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G96">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
+      <c r="L96">
+        <v>0</v>
+      </c>
+      <c r="M96">
+        <v>0</v>
+      </c>
+      <c r="N96">
+        <v>0</v>
+      </c>
+      <c r="O96">
+        <v>1</v>
+      </c>
+      <c r="P96">
+        <v>0</v>
+      </c>
+      <c r="Q96">
+        <v>0</v>
+      </c>
+      <c r="R96">
+        <v>1</v>
+      </c>
+      <c r="S96">
+        <v>0</v>
+      </c>
+      <c r="T96">
+        <v>0</v>
+      </c>
+      <c r="U96">
+        <v>1</v>
+      </c>
+      <c r="V96">
+        <v>1</v>
+      </c>
+      <c r="W96">
+        <v>1</v>
+      </c>
+      <c r="X96">
+        <v>0</v>
+      </c>
+      <c r="Y96">
+        <v>1</v>
+      </c>
+      <c r="Z96">
+        <v>0</v>
+      </c>
+      <c r="AA96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>142</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="C97" t="s">
+        <v>121</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="L97">
+        <v>0</v>
+      </c>
+      <c r="M97">
+        <v>0</v>
+      </c>
+      <c r="N97">
+        <v>0</v>
+      </c>
+      <c r="O97">
+        <v>0</v>
+      </c>
+      <c r="P97">
+        <v>0</v>
+      </c>
+      <c r="Q97">
+        <v>1</v>
+      </c>
+      <c r="R97">
+        <v>1</v>
+      </c>
+      <c r="S97">
+        <v>1</v>
+      </c>
+      <c r="T97">
+        <v>1</v>
+      </c>
+      <c r="U97">
+        <v>1</v>
+      </c>
+      <c r="V97">
+        <v>1</v>
+      </c>
+      <c r="W97">
+        <v>1</v>
+      </c>
+      <c r="X97">
+        <v>0</v>
+      </c>
+      <c r="Y97">
+        <v>0</v>
+      </c>
+      <c r="Z97">
+        <v>1</v>
+      </c>
+      <c r="AA97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>129</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="C98" t="s">
+        <v>121</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G98">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98">
+        <v>0</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <v>0</v>
+      </c>
+      <c r="M98">
+        <v>0</v>
+      </c>
+      <c r="N98">
+        <v>0</v>
+      </c>
+      <c r="O98">
+        <v>0</v>
+      </c>
+      <c r="P98">
+        <v>0</v>
+      </c>
+      <c r="Q98">
+        <v>0</v>
+      </c>
+      <c r="R98">
+        <v>0</v>
+      </c>
+      <c r="S98">
+        <v>0</v>
+      </c>
+      <c r="T98">
+        <v>1</v>
+      </c>
+      <c r="U98">
+        <v>1</v>
+      </c>
+      <c r="V98">
+        <v>0</v>
+      </c>
+      <c r="W98">
+        <v>1</v>
+      </c>
+      <c r="X98">
+        <v>1</v>
+      </c>
+      <c r="Y98">
+        <v>1</v>
+      </c>
+      <c r="Z98">
+        <v>1</v>
+      </c>
+      <c r="AA98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>130</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="C99" t="s">
+        <v>121</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G99">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="I99">
+        <v>0</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+      <c r="K99">
+        <v>0</v>
+      </c>
+      <c r="L99">
+        <v>0</v>
+      </c>
+      <c r="M99">
+        <v>0</v>
+      </c>
+      <c r="N99">
+        <v>0</v>
+      </c>
+      <c r="O99">
+        <v>0</v>
+      </c>
+      <c r="P99">
+        <v>0</v>
+      </c>
+      <c r="Q99">
+        <v>0</v>
+      </c>
+      <c r="R99">
+        <v>1</v>
+      </c>
+      <c r="S99">
+        <v>0</v>
+      </c>
+      <c r="T99">
+        <v>1</v>
+      </c>
+      <c r="U99">
+        <v>1</v>
+      </c>
+      <c r="V99">
+        <v>1</v>
+      </c>
+      <c r="W99">
+        <v>1</v>
+      </c>
+      <c r="X99">
+        <v>1</v>
+      </c>
+      <c r="Y99">
+        <v>0</v>
+      </c>
+      <c r="Z99">
+        <v>1</v>
+      </c>
+      <c r="AA99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>131</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="C100" t="s">
+        <v>121</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G100">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H100">
+        <v>1</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+      <c r="K100">
+        <v>1</v>
+      </c>
+      <c r="L100">
+        <v>1</v>
+      </c>
+      <c r="M100">
+        <v>1</v>
+      </c>
+      <c r="N100">
+        <v>1</v>
+      </c>
+      <c r="O100">
+        <v>0</v>
+      </c>
+      <c r="P100">
+        <v>0</v>
+      </c>
+      <c r="Q100">
+        <v>0</v>
+      </c>
+      <c r="R100">
+        <v>1</v>
+      </c>
+      <c r="S100">
+        <v>0</v>
+      </c>
+      <c r="T100">
+        <v>0</v>
+      </c>
+      <c r="U100">
+        <v>1</v>
+      </c>
+      <c r="V100">
+        <v>1</v>
+      </c>
+      <c r="W100">
+        <v>1</v>
+      </c>
+      <c r="X100">
+        <v>1</v>
+      </c>
+      <c r="Y100">
+        <v>1</v>
+      </c>
+      <c r="Z100">
+        <v>1</v>
+      </c>
+      <c r="AA100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>141</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="C101" t="s">
+        <v>121</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="G101">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101">
+        <v>0</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
+      </c>
+      <c r="K101">
+        <v>1</v>
+      </c>
+      <c r="L101">
+        <v>1</v>
+      </c>
+      <c r="M101">
+        <v>0</v>
+      </c>
+      <c r="N101">
+        <v>0</v>
+      </c>
+      <c r="O101">
+        <v>0</v>
+      </c>
+      <c r="P101">
+        <v>0</v>
+      </c>
+      <c r="Q101">
+        <v>0</v>
+      </c>
+      <c r="R101">
+        <v>0</v>
+      </c>
+      <c r="S101">
+        <v>0</v>
+      </c>
+      <c r="T101">
+        <v>1</v>
+      </c>
+      <c r="U101">
+        <v>1</v>
+      </c>
+      <c r="V101">
+        <v>1</v>
+      </c>
+      <c r="W101">
+        <v>1</v>
+      </c>
+      <c r="X101">
+        <v>1</v>
+      </c>
+      <c r="Y101">
+        <v>1</v>
+      </c>
+      <c r="Z101">
+        <v>1</v>
+      </c>
+      <c r="AA101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>132</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="C102" t="s">
+        <v>121</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G102">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+      <c r="I102">
+        <v>1</v>
+      </c>
+      <c r="J102">
+        <v>1</v>
+      </c>
+      <c r="K102">
+        <v>0</v>
+      </c>
+      <c r="L102">
+        <v>0</v>
+      </c>
+      <c r="M102">
+        <v>0</v>
+      </c>
+      <c r="N102">
+        <v>0</v>
+      </c>
+      <c r="O102">
+        <v>0</v>
+      </c>
+      <c r="P102">
+        <v>0</v>
+      </c>
+      <c r="Q102">
+        <v>0</v>
+      </c>
+      <c r="R102">
+        <v>1</v>
+      </c>
+      <c r="S102">
+        <v>0</v>
+      </c>
+      <c r="T102">
+        <v>1</v>
+      </c>
+      <c r="U102">
+        <v>1</v>
+      </c>
+      <c r="V102">
+        <v>1</v>
+      </c>
+      <c r="W102">
+        <v>1</v>
+      </c>
+      <c r="X102">
+        <v>1</v>
+      </c>
+      <c r="Y102">
+        <v>0</v>
+      </c>
+      <c r="Z102">
+        <v>1</v>
+      </c>
+      <c r="AA102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>133</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="C103" t="s">
+        <v>121</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="G103">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H103">
+        <v>0</v>
+      </c>
+      <c r="I103">
+        <v>0</v>
+      </c>
+      <c r="J103">
+        <v>0</v>
+      </c>
+      <c r="K103">
+        <v>0</v>
+      </c>
+      <c r="L103">
+        <v>0</v>
+      </c>
+      <c r="M103">
+        <v>0</v>
+      </c>
+      <c r="N103">
+        <v>0</v>
+      </c>
+      <c r="O103">
+        <v>0</v>
+      </c>
+      <c r="P103">
+        <v>0</v>
+      </c>
+      <c r="Q103">
+        <v>0</v>
+      </c>
+      <c r="R103">
+        <v>1</v>
+      </c>
+      <c r="S103">
+        <v>0</v>
+      </c>
+      <c r="T103">
+        <v>1</v>
+      </c>
+      <c r="U103">
+        <v>1</v>
+      </c>
+      <c r="V103">
+        <v>1</v>
+      </c>
+      <c r="W103">
+        <v>1</v>
+      </c>
+      <c r="X103">
+        <v>1</v>
+      </c>
+      <c r="Y103">
+        <v>1</v>
+      </c>
+      <c r="Z103">
+        <v>1</v>
+      </c>
+      <c r="AA103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>134</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="C104" t="s">
+        <v>121</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="F104">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="G104">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="H104">
+        <v>1</v>
+      </c>
+      <c r="I104">
+        <v>1</v>
+      </c>
+      <c r="J104">
+        <v>1</v>
+      </c>
+      <c r="K104">
+        <v>0</v>
+      </c>
+      <c r="L104">
+        <v>0</v>
+      </c>
+      <c r="M104">
+        <v>0</v>
+      </c>
+      <c r="N104">
+        <v>0</v>
+      </c>
+      <c r="O104">
+        <v>0</v>
+      </c>
+      <c r="P104">
+        <v>1</v>
+      </c>
+      <c r="Q104">
+        <v>1</v>
+      </c>
+      <c r="R104">
+        <v>1</v>
+      </c>
+      <c r="S104">
+        <v>0</v>
+      </c>
+      <c r="T104">
+        <v>1</v>
+      </c>
+      <c r="U104">
+        <v>1</v>
+      </c>
+      <c r="V104">
+        <v>1</v>
+      </c>
+      <c r="W104">
+        <v>1</v>
+      </c>
+      <c r="X104">
+        <v>1</v>
+      </c>
+      <c r="Y104">
+        <v>1</v>
+      </c>
+      <c r="Z104">
+        <v>1</v>
+      </c>
+      <c r="AA104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>135</v>
+      </c>
+      <c r="B105">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="C105" t="s">
+        <v>121</v>
+      </c>
+      <c r="D105">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="G105">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H105">
+        <v>1</v>
+      </c>
+      <c r="I105">
+        <v>0</v>
+      </c>
+      <c r="J105">
+        <v>0</v>
+      </c>
+      <c r="K105">
+        <v>0</v>
+      </c>
+      <c r="L105">
+        <v>0</v>
+      </c>
+      <c r="M105">
+        <v>0</v>
+      </c>
+      <c r="N105">
+        <v>0</v>
+      </c>
+      <c r="O105">
+        <v>1</v>
+      </c>
+      <c r="P105">
+        <v>0</v>
+      </c>
+      <c r="Q105">
+        <v>0</v>
+      </c>
+      <c r="R105">
+        <v>1</v>
+      </c>
+      <c r="S105">
+        <v>0</v>
+      </c>
+      <c r="T105">
+        <v>1</v>
+      </c>
+      <c r="U105">
+        <v>1</v>
+      </c>
+      <c r="V105">
+        <v>0</v>
+      </c>
+      <c r="W105">
+        <v>0</v>
+      </c>
+      <c r="X105">
+        <v>0</v>
+      </c>
+      <c r="Y105">
+        <v>0</v>
+      </c>
+      <c r="Z105">
+        <v>1</v>
+      </c>
+      <c r="AA105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>136</v>
+      </c>
+      <c r="B106">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="C106" t="s">
+        <v>121</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F106">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G106">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H106">
+        <v>1</v>
+      </c>
+      <c r="I106">
+        <v>0</v>
+      </c>
+      <c r="J106">
+        <v>0</v>
+      </c>
+      <c r="K106">
+        <v>1</v>
+      </c>
+      <c r="L106">
+        <v>1</v>
+      </c>
+      <c r="M106">
+        <v>0</v>
+      </c>
+      <c r="N106">
+        <v>0</v>
+      </c>
+      <c r="O106">
+        <v>0</v>
+      </c>
+      <c r="P106">
+        <v>0</v>
+      </c>
+      <c r="Q106">
+        <v>0</v>
+      </c>
+      <c r="R106">
+        <v>1</v>
+      </c>
+      <c r="S106">
+        <v>0</v>
+      </c>
+      <c r="T106">
+        <v>0</v>
+      </c>
+      <c r="U106">
+        <v>1</v>
+      </c>
+      <c r="V106">
+        <v>1</v>
+      </c>
+      <c r="W106">
+        <v>1</v>
+      </c>
+      <c r="X106">
+        <v>1</v>
+      </c>
+      <c r="Y106">
+        <v>0</v>
+      </c>
+      <c r="Z106">
+        <v>1</v>
+      </c>
+      <c r="AA106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>137</v>
+      </c>
+      <c r="B107">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="C107" t="s">
+        <v>121</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="F107">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="G107">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H107">
+        <v>1</v>
+      </c>
+      <c r="I107">
+        <v>0</v>
+      </c>
+      <c r="J107">
+        <v>0</v>
+      </c>
+      <c r="K107">
+        <v>0</v>
+      </c>
+      <c r="L107">
+        <v>0</v>
+      </c>
+      <c r="M107">
+        <v>0</v>
+      </c>
+      <c r="N107">
+        <v>0</v>
+      </c>
+      <c r="O107">
+        <v>0</v>
+      </c>
+      <c r="P107">
+        <v>0</v>
+      </c>
+      <c r="Q107">
+        <v>0</v>
+      </c>
+      <c r="R107">
+        <v>0</v>
+      </c>
+      <c r="S107">
+        <v>0</v>
+      </c>
+      <c r="T107">
+        <v>0</v>
+      </c>
+      <c r="U107">
+        <v>0</v>
+      </c>
+      <c r="V107">
+        <v>0</v>
+      </c>
+      <c r="W107">
+        <v>0</v>
+      </c>
+      <c r="X107">
+        <v>0</v>
+      </c>
+      <c r="Y107">
+        <v>1</v>
+      </c>
+      <c r="Z107">
+        <v>1</v>
+      </c>
+      <c r="AA107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>138</v>
+      </c>
+      <c r="B108">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="C108" t="s">
+        <v>121</v>
+      </c>
+      <c r="D108">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="E108">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F108">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G108">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H108">
+        <v>1</v>
+      </c>
+      <c r="I108">
+        <v>1</v>
+      </c>
+      <c r="J108">
+        <v>1</v>
+      </c>
+      <c r="K108">
+        <v>0</v>
+      </c>
+      <c r="L108">
+        <v>0</v>
+      </c>
+      <c r="M108">
+        <v>0</v>
+      </c>
+      <c r="N108">
+        <v>0</v>
+      </c>
+      <c r="O108">
+        <v>0</v>
+      </c>
+      <c r="P108">
+        <v>0</v>
+      </c>
+      <c r="Q108">
+        <v>0</v>
+      </c>
+      <c r="R108">
+        <v>1</v>
+      </c>
+      <c r="S108">
+        <v>0</v>
+      </c>
+      <c r="T108">
+        <v>1</v>
+      </c>
+      <c r="U108">
+        <v>0</v>
+      </c>
+      <c r="V108">
+        <v>1</v>
+      </c>
+      <c r="W108">
+        <v>1</v>
+      </c>
+      <c r="X108">
+        <v>1</v>
+      </c>
+      <c r="Y108">
+        <v>1</v>
+      </c>
+      <c r="Z108">
+        <v>1</v>
+      </c>
+      <c r="AA108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>139</v>
+      </c>
+      <c r="B109">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="C109" t="s">
+        <v>121</v>
+      </c>
+      <c r="D109">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E109">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G109">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="H109">
+        <v>1</v>
+      </c>
+      <c r="I109">
+        <v>0</v>
+      </c>
+      <c r="J109">
+        <v>0</v>
+      </c>
+      <c r="K109">
+        <v>0</v>
+      </c>
+      <c r="L109">
+        <v>1</v>
+      </c>
+      <c r="M109">
+        <v>0</v>
+      </c>
+      <c r="N109">
+        <v>0</v>
+      </c>
+      <c r="O109">
+        <v>0</v>
+      </c>
+      <c r="P109">
+        <v>0</v>
+      </c>
+      <c r="Q109">
+        <v>0</v>
+      </c>
+      <c r="R109">
+        <v>1</v>
+      </c>
+      <c r="S109">
+        <v>0</v>
+      </c>
+      <c r="T109">
+        <v>1</v>
+      </c>
+      <c r="U109">
+        <v>1</v>
+      </c>
+      <c r="V109">
+        <v>1</v>
+      </c>
+      <c r="W109">
+        <v>1</v>
+      </c>
+      <c r="X109">
+        <v>0</v>
+      </c>
+      <c r="Y109">
+        <v>1</v>
+      </c>
+      <c r="Z109">
+        <v>1</v>
+      </c>
+      <c r="AA109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>140</v>
+      </c>
+      <c r="B110">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="C110" t="s">
+        <v>121</v>
+      </c>
+      <c r="D110">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E110">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="G110">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="H110">
+        <v>1</v>
+      </c>
+      <c r="I110">
+        <v>0</v>
+      </c>
+      <c r="J110">
+        <v>0</v>
+      </c>
+      <c r="K110">
+        <v>0</v>
+      </c>
+      <c r="L110">
+        <v>0</v>
+      </c>
+      <c r="M110">
+        <v>0</v>
+      </c>
+      <c r="N110">
+        <v>0</v>
+      </c>
+      <c r="O110">
+        <v>1</v>
+      </c>
+      <c r="P110">
+        <v>1</v>
+      </c>
+      <c r="Q110">
+        <v>1</v>
+      </c>
+      <c r="R110">
+        <v>1</v>
+      </c>
+      <c r="S110">
+        <v>1</v>
+      </c>
+      <c r="T110">
+        <v>1</v>
+      </c>
+      <c r="U110">
+        <v>1</v>
+      </c>
+      <c r="V110">
+        <v>1</v>
+      </c>
+      <c r="W110">
+        <v>1</v>
+      </c>
+      <c r="X110">
+        <v>1</v>
+      </c>
+      <c r="Y110">
+        <v>1</v>
+      </c>
+      <c r="Z110">
+        <v>1</v>
+      </c>
+      <c r="AA110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>144</v>
+      </c>
+      <c r="B111">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="C111" t="s">
+        <v>143</v>
+      </c>
+      <c r="D111">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E111">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="G111">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H111">
+        <v>0</v>
+      </c>
+      <c r="I111">
+        <v>0</v>
+      </c>
+      <c r="J111">
+        <v>0</v>
+      </c>
+      <c r="K111">
+        <v>0</v>
+      </c>
+      <c r="L111">
+        <v>0</v>
+      </c>
+      <c r="M111">
+        <v>0</v>
+      </c>
+      <c r="N111">
+        <v>0</v>
+      </c>
+      <c r="O111">
+        <v>0</v>
+      </c>
+      <c r="P111">
+        <v>0</v>
+      </c>
+      <c r="Q111">
+        <v>0</v>
+      </c>
+      <c r="R111">
+        <v>1</v>
+      </c>
+      <c r="S111">
+        <v>0</v>
+      </c>
+      <c r="T111">
+        <v>1</v>
+      </c>
+      <c r="U111">
+        <v>1</v>
+      </c>
+      <c r="V111">
+        <v>1</v>
+      </c>
+      <c r="W111">
+        <v>1</v>
+      </c>
+      <c r="X111">
+        <v>1</v>
+      </c>
+      <c r="Y111">
+        <v>1</v>
+      </c>
+      <c r="Z111">
+        <v>1</v>
+      </c>
+      <c r="AA111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>145</v>
+      </c>
+      <c r="B112">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="C112" t="s">
+        <v>143</v>
+      </c>
+      <c r="D112">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E112">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G112">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H112">
+        <v>0</v>
+      </c>
+      <c r="I112">
+        <v>0</v>
+      </c>
+      <c r="J112">
+        <v>0</v>
+      </c>
+      <c r="K112">
+        <v>0</v>
+      </c>
+      <c r="L112">
+        <v>0</v>
+      </c>
+      <c r="M112">
+        <v>0</v>
+      </c>
+      <c r="N112">
+        <v>0</v>
+      </c>
+      <c r="O112">
+        <v>1</v>
+      </c>
+      <c r="P112">
+        <v>0</v>
+      </c>
+      <c r="Q112">
+        <v>0</v>
+      </c>
+      <c r="R112">
+        <v>1</v>
+      </c>
+      <c r="S112">
+        <v>0</v>
+      </c>
+      <c r="T112">
+        <v>1</v>
+      </c>
+      <c r="U112">
+        <v>1</v>
+      </c>
+      <c r="V112">
+        <v>0</v>
+      </c>
+      <c r="W112">
+        <v>0</v>
+      </c>
+      <c r="X112">
+        <v>1</v>
+      </c>
+      <c r="Y112">
+        <v>1</v>
+      </c>
+      <c r="Z112">
+        <v>1</v>
+      </c>
+      <c r="AA112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>146</v>
+      </c>
+      <c r="B113" s="1">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="C113" t="s">
+        <v>143</v>
+      </c>
+      <c r="D113" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E113" s="1">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G113">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H113">
+        <v>0</v>
+      </c>
+      <c r="I113">
+        <v>0</v>
+      </c>
+      <c r="J113">
+        <v>0</v>
+      </c>
+      <c r="K113">
+        <v>0</v>
+      </c>
+      <c r="L113">
+        <v>0</v>
+      </c>
+      <c r="M113">
+        <v>0</v>
+      </c>
+      <c r="N113">
+        <v>0</v>
+      </c>
+      <c r="O113">
+        <v>0</v>
+      </c>
+      <c r="P113">
+        <v>0</v>
+      </c>
+      <c r="Q113">
+        <v>0</v>
+      </c>
+      <c r="R113">
+        <v>1</v>
+      </c>
+      <c r="S113">
+        <v>0</v>
+      </c>
+      <c r="T113">
+        <v>0</v>
+      </c>
+      <c r="U113">
+        <v>1</v>
+      </c>
+      <c r="V113">
+        <v>1</v>
+      </c>
+      <c r="W113">
+        <v>1</v>
+      </c>
+      <c r="X113">
+        <v>1</v>
+      </c>
+      <c r="Y113">
+        <v>0</v>
+      </c>
+      <c r="Z113">
+        <v>1</v>
+      </c>
+      <c r="AA113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>147</v>
+      </c>
+      <c r="B114" s="1">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="C114" t="s">
+        <v>143</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G114">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H114">
+        <v>0</v>
+      </c>
+      <c r="I114">
+        <v>0</v>
+      </c>
+      <c r="J114">
+        <v>0</v>
+      </c>
+      <c r="K114">
+        <v>0</v>
+      </c>
+      <c r="L114">
+        <v>0</v>
+      </c>
+      <c r="M114">
+        <v>0</v>
+      </c>
+      <c r="N114">
+        <v>0</v>
+      </c>
+      <c r="O114">
+        <v>0</v>
+      </c>
+      <c r="P114">
+        <v>0</v>
+      </c>
+      <c r="Q114">
+        <v>0</v>
+      </c>
+      <c r="R114">
+        <v>0</v>
+      </c>
+      <c r="S114">
+        <v>0</v>
+      </c>
+      <c r="T114">
+        <v>0</v>
+      </c>
+      <c r="U114">
+        <v>1</v>
+      </c>
+      <c r="V114">
+        <v>1</v>
+      </c>
+      <c r="W114">
+        <v>1</v>
+      </c>
+      <c r="X114">
+        <v>1</v>
+      </c>
+      <c r="Y114">
+        <v>1</v>
+      </c>
+      <c r="Z114">
+        <v>1</v>
+      </c>
+      <c r="AA114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>148</v>
+      </c>
+      <c r="B115" s="1">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="C115" t="s">
+        <v>143</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="G115">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="H115">
+        <v>0</v>
+      </c>
+      <c r="I115">
+        <v>0</v>
+      </c>
+      <c r="J115">
+        <v>0</v>
+      </c>
+      <c r="K115">
+        <v>0</v>
+      </c>
+      <c r="L115">
+        <v>0</v>
+      </c>
+      <c r="M115">
+        <v>0</v>
+      </c>
+      <c r="N115">
+        <v>0</v>
+      </c>
+      <c r="O115">
+        <v>0</v>
+      </c>
+      <c r="P115">
+        <v>0</v>
+      </c>
+      <c r="Q115">
+        <v>0</v>
+      </c>
+      <c r="R115">
+        <v>0</v>
+      </c>
+      <c r="S115">
+        <v>0</v>
+      </c>
+      <c r="T115">
+        <v>1</v>
+      </c>
+      <c r="U115">
+        <v>0</v>
+      </c>
+      <c r="V115">
+        <v>0</v>
+      </c>
+      <c r="W115">
+        <v>0</v>
+      </c>
+      <c r="X115">
+        <v>0</v>
+      </c>
+      <c r="Y115">
+        <v>1</v>
+      </c>
+      <c r="Z115">
+        <v>1</v>
+      </c>
+      <c r="AA115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>149</v>
+      </c>
+      <c r="B116" s="1">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="C116" t="s">
+        <v>143</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E116">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G116">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H116">
+        <v>1</v>
+      </c>
+      <c r="I116">
+        <v>0</v>
+      </c>
+      <c r="J116">
+        <v>0</v>
+      </c>
+      <c r="K116">
+        <v>0</v>
+      </c>
+      <c r="L116">
+        <v>0</v>
+      </c>
+      <c r="M116">
+        <v>0</v>
+      </c>
+      <c r="N116">
+        <v>0</v>
+      </c>
+      <c r="O116">
+        <v>0</v>
+      </c>
+      <c r="P116">
+        <v>0</v>
+      </c>
+      <c r="Q116">
+        <v>0</v>
+      </c>
+      <c r="R116">
+        <v>0</v>
+      </c>
+      <c r="S116">
+        <v>0</v>
+      </c>
+      <c r="T116">
+        <v>1</v>
+      </c>
+      <c r="U116">
+        <v>0</v>
+      </c>
+      <c r="V116">
+        <v>1</v>
+      </c>
+      <c r="W116">
+        <v>1</v>
+      </c>
+      <c r="X116">
+        <v>1</v>
+      </c>
+      <c r="Y116">
+        <v>1</v>
+      </c>
+      <c r="Z116">
+        <v>1</v>
+      </c>
+      <c r="AA116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>150</v>
+      </c>
+      <c r="B117" s="1">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="C117" t="s">
+        <v>143</v>
+      </c>
+      <c r="D117">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="E117">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G117">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H117">
+        <v>1</v>
+      </c>
+      <c r="I117">
+        <v>0</v>
+      </c>
+      <c r="J117">
+        <v>0</v>
+      </c>
+      <c r="K117">
+        <v>1</v>
+      </c>
+      <c r="L117">
+        <v>1</v>
+      </c>
+      <c r="M117">
+        <v>0</v>
+      </c>
+      <c r="N117">
+        <v>0</v>
+      </c>
+      <c r="O117">
+        <v>0</v>
+      </c>
+      <c r="P117">
+        <v>0</v>
+      </c>
+      <c r="Q117">
+        <v>0</v>
+      </c>
+      <c r="R117">
+        <v>1</v>
+      </c>
+      <c r="S117">
+        <v>0</v>
+      </c>
+      <c r="T117">
+        <v>1</v>
+      </c>
+      <c r="U117">
+        <v>1</v>
+      </c>
+      <c r="V117">
+        <v>0</v>
+      </c>
+      <c r="W117">
+        <v>1</v>
+      </c>
+      <c r="X117">
+        <v>1</v>
+      </c>
+      <c r="Y117">
+        <v>1</v>
+      </c>
+      <c r="Z117">
+        <v>1</v>
+      </c>
+      <c r="AA117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>151</v>
+      </c>
+      <c r="B118" s="1">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="C118" t="s">
+        <v>143</v>
+      </c>
+      <c r="D118">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E118">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="G118">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H118">
+        <v>1</v>
+      </c>
+      <c r="I118">
+        <v>0</v>
+      </c>
+      <c r="J118">
+        <v>0</v>
+      </c>
+      <c r="K118">
+        <v>0</v>
+      </c>
+      <c r="L118">
+        <v>0</v>
+      </c>
+      <c r="M118">
+        <v>0</v>
+      </c>
+      <c r="N118">
+        <v>0</v>
+      </c>
+      <c r="O118">
+        <v>1</v>
+      </c>
+      <c r="P118">
+        <v>0</v>
+      </c>
+      <c r="Q118">
+        <v>0</v>
+      </c>
+      <c r="R118">
+        <v>1</v>
+      </c>
+      <c r="S118">
+        <v>0</v>
+      </c>
+      <c r="T118">
+        <v>0</v>
+      </c>
+      <c r="U118">
+        <v>1</v>
+      </c>
+      <c r="V118">
+        <v>0</v>
+      </c>
+      <c r="W118">
+        <v>0</v>
+      </c>
+      <c r="X118">
+        <v>0</v>
+      </c>
+      <c r="Y118">
+        <v>0</v>
+      </c>
+      <c r="Z118">
+        <v>1</v>
+      </c>
+      <c r="AA118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>152</v>
+      </c>
+      <c r="B119" s="1">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="C119" t="s">
+        <v>143</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E119">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G119">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H119">
+        <v>0</v>
+      </c>
+      <c r="I119">
+        <v>0</v>
+      </c>
+      <c r="J119">
+        <v>0</v>
+      </c>
+      <c r="K119">
+        <v>0</v>
+      </c>
+      <c r="L119">
+        <v>0</v>
+      </c>
+      <c r="M119">
+        <v>0</v>
+      </c>
+      <c r="N119">
+        <v>0</v>
+      </c>
+      <c r="O119">
+        <v>0</v>
+      </c>
+      <c r="P119">
+        <v>1</v>
+      </c>
+      <c r="Q119">
+        <v>0</v>
+      </c>
+      <c r="R119">
+        <v>0</v>
+      </c>
+      <c r="S119">
+        <v>1</v>
+      </c>
+      <c r="T119">
+        <v>1</v>
+      </c>
+      <c r="U119">
+        <v>1</v>
+      </c>
+      <c r="V119">
+        <v>1</v>
+      </c>
+      <c r="W119">
+        <v>1</v>
+      </c>
+      <c r="X119">
+        <v>0</v>
+      </c>
+      <c r="Y119">
+        <v>0</v>
+      </c>
+      <c r="Z119">
+        <v>1</v>
+      </c>
+      <c r="AA119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>153</v>
+      </c>
+      <c r="B120" s="1">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="C120" t="s">
+        <v>143</v>
+      </c>
+      <c r="D120">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E120">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G120">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H120">
+        <v>1</v>
+      </c>
+      <c r="I120">
+        <v>0</v>
+      </c>
+      <c r="J120">
+        <v>0</v>
+      </c>
+      <c r="K120">
+        <v>0</v>
+      </c>
+      <c r="L120">
+        <v>0</v>
+      </c>
+      <c r="M120">
+        <v>0</v>
+      </c>
+      <c r="N120">
+        <v>0</v>
+      </c>
+      <c r="O120">
+        <v>0</v>
+      </c>
+      <c r="P120">
+        <v>0</v>
+      </c>
+      <c r="Q120">
+        <v>0</v>
+      </c>
+      <c r="R120">
+        <v>1</v>
+      </c>
+      <c r="S120">
+        <v>0</v>
+      </c>
+      <c r="T120">
+        <v>0</v>
+      </c>
+      <c r="U120">
+        <v>0</v>
+      </c>
+      <c r="V120">
+        <v>1</v>
+      </c>
+      <c r="W120">
+        <v>1</v>
+      </c>
+      <c r="X120">
+        <v>1</v>
+      </c>
+      <c r="Y120">
+        <v>1</v>
+      </c>
+      <c r="Z120">
+        <v>1</v>
+      </c>
+      <c r="AA120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>154</v>
+      </c>
+      <c r="B121" s="1">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="C121" t="s">
+        <v>143</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E121">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G121">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H121">
+        <v>0</v>
+      </c>
+      <c r="I121">
+        <v>0</v>
+      </c>
+      <c r="J121">
+        <v>0</v>
+      </c>
+      <c r="K121">
+        <v>0</v>
+      </c>
+      <c r="L121">
+        <v>0</v>
+      </c>
+      <c r="M121">
+        <v>0</v>
+      </c>
+      <c r="N121">
+        <v>0</v>
+      </c>
+      <c r="O121">
+        <v>0</v>
+      </c>
+      <c r="P121">
+        <v>0</v>
+      </c>
+      <c r="Q121">
+        <v>0</v>
+      </c>
+      <c r="R121">
+        <v>1</v>
+      </c>
+      <c r="S121">
+        <v>1</v>
+      </c>
+      <c r="T121">
+        <v>0</v>
+      </c>
+      <c r="U121">
+        <v>1</v>
+      </c>
+      <c r="V121">
+        <v>0</v>
+      </c>
+      <c r="W121">
+        <v>1</v>
+      </c>
+      <c r="X121">
+        <v>1</v>
+      </c>
+      <c r="Y121">
+        <v>1</v>
+      </c>
+      <c r="Z121">
+        <v>1</v>
+      </c>
+      <c r="AA121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>155</v>
+      </c>
+      <c r="B122" s="1">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="C122" t="s">
+        <v>143</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="G122">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H122">
+        <v>0</v>
+      </c>
+      <c r="I122">
+        <v>0</v>
+      </c>
+      <c r="J122">
+        <v>0</v>
+      </c>
+      <c r="K122">
+        <v>0</v>
+      </c>
+      <c r="L122">
+        <v>0</v>
+      </c>
+      <c r="M122">
+        <v>0</v>
+      </c>
+      <c r="N122">
+        <v>0</v>
+      </c>
+      <c r="O122">
+        <v>0</v>
+      </c>
+      <c r="P122">
+        <v>0</v>
+      </c>
+      <c r="Q122">
+        <v>0</v>
+      </c>
+      <c r="R122">
+        <v>0</v>
+      </c>
+      <c r="S122">
+        <v>0</v>
+      </c>
+      <c r="T122">
+        <v>1</v>
+      </c>
+      <c r="U122">
+        <v>1</v>
+      </c>
+      <c r="V122">
+        <v>1</v>
+      </c>
+      <c r="W122">
+        <v>1</v>
+      </c>
+      <c r="X122">
+        <v>1</v>
+      </c>
+      <c r="Y122">
+        <v>1</v>
+      </c>
+      <c r="Z122">
+        <v>1</v>
+      </c>
+      <c r="AA122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>156</v>
+      </c>
+      <c r="B123" s="1">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="C123" t="s">
+        <v>143</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E123">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="G123">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H123">
+        <v>1</v>
+      </c>
+      <c r="I123">
+        <v>0</v>
+      </c>
+      <c r="J123">
+        <v>0</v>
+      </c>
+      <c r="K123">
+        <v>0</v>
+      </c>
+      <c r="L123">
+        <v>0</v>
+      </c>
+      <c r="M123">
+        <v>0</v>
+      </c>
+      <c r="N123">
+        <v>0</v>
+      </c>
+      <c r="O123">
+        <v>0</v>
+      </c>
+      <c r="P123">
+        <v>0</v>
+      </c>
+      <c r="Q123">
+        <v>0</v>
+      </c>
+      <c r="R123">
+        <v>1</v>
+      </c>
+      <c r="S123">
+        <v>0</v>
+      </c>
+      <c r="T123">
+        <v>0</v>
+      </c>
+      <c r="U123">
+        <v>0</v>
+      </c>
+      <c r="V123">
+        <v>0</v>
+      </c>
+      <c r="W123">
+        <v>0</v>
+      </c>
+      <c r="X123">
+        <v>0</v>
+      </c>
+      <c r="Y123">
+        <v>1</v>
+      </c>
+      <c r="Z123">
+        <v>1</v>
+      </c>
+      <c r="AA123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>157</v>
+      </c>
+      <c r="B124" s="1">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="C124" t="s">
+        <v>143</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E124">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G124">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="H124">
+        <v>1</v>
+      </c>
+      <c r="I124">
+        <v>0</v>
+      </c>
+      <c r="J124">
+        <v>0</v>
+      </c>
+      <c r="K124">
+        <v>0</v>
+      </c>
+      <c r="L124">
+        <v>1</v>
+      </c>
+      <c r="M124">
+        <v>0</v>
+      </c>
+      <c r="N124">
+        <v>0</v>
+      </c>
+      <c r="O124">
+        <v>0</v>
+      </c>
+      <c r="P124">
+        <v>0</v>
+      </c>
+      <c r="Q124">
+        <v>0</v>
+      </c>
+      <c r="R124">
+        <v>1</v>
+      </c>
+      <c r="S124">
+        <v>0</v>
+      </c>
+      <c r="T124">
+        <v>1</v>
+      </c>
+      <c r="U124">
+        <v>1</v>
+      </c>
+      <c r="V124">
+        <v>0</v>
+      </c>
+      <c r="W124">
+        <v>1</v>
+      </c>
+      <c r="X124">
+        <v>1</v>
+      </c>
+      <c r="Y124">
+        <v>1</v>
+      </c>
+      <c r="Z124">
+        <v>1</v>
+      </c>
+      <c r="AA124">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>